<commit_message>
dodanie logowania rozmiaru pamięci
</commit_message>
<xml_diff>
--- a/Programowanie współbieżne/resources/Zadanie 7.xlsx
+++ b/Programowanie współbieżne/resources/Zadanie 7.xlsx
@@ -74,6 +74,174 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="539525696"/>
+        <c:axId val="54811968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="539525696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54811968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54811968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539525696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +546,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,8 +702,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
zadanie skończone i sprawko napisane
</commit_message>
<xml_diff>
--- a/Programowanie współbieżne/resources/Zadanie 7.xlsx
+++ b/Programowanie współbieżne/resources/Zadanie 7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="6735"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="6735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>węzły</t>
   </si>
@@ -25,6 +25,24 @@
   </si>
   <si>
     <t>czas</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>reponse</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>sent to node</t>
+  </si>
+  <si>
+    <t>sent to client</t>
+  </si>
+  <si>
+    <t>total data</t>
   </si>
 </sst>
 </file>
@@ -66,7 +84,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -157,11 +185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539525696"/>
-        <c:axId val="54811968"/>
+        <c:axId val="503436928"/>
+        <c:axId val="503437504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539525696"/>
+        <c:axId val="503436928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -171,12 +199,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54811968"/>
+        <c:crossAx val="503437504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54811968"/>
+        <c:axId val="503437504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -187,7 +215,149 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539525696"/>
+        <c:crossAx val="503436928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>39887348</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48296936</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65116112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98754464</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="571987008"/>
+        <c:axId val="571986432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="571987008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="571986432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="571986432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="571987008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -244,6 +414,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>690562</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
   <autoFilter ref="A1:C16"/>
@@ -251,6 +456,27 @@
     <tableColumn id="1" name="węzły"/>
     <tableColumn id="2" name="N"/>
     <tableColumn id="3" name="czas"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="3" name="nodes"/>
+    <tableColumn id="1" name="request"/>
+    <tableColumn id="4" name="sent to node" dataDxfId="2">
+      <calculatedColumnFormula>Table2[request]*Table2[nodes]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="reponse"/>
+    <tableColumn id="5" name="sent to client" dataDxfId="1">
+      <calculatedColumnFormula>Table2[reponse]*Table2[nodes]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="total data" dataDxfId="0">
+      <calculatedColumnFormula>Table2[sent to node]+Table2[sent to client]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -545,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
@@ -711,13 +937,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>16818438</v>
+      </c>
+      <c r="C2">
+        <f>Table2[request]*Table2[nodes]</f>
+        <v>16818438</v>
+      </c>
+      <c r="D2">
+        <v>23068910</v>
+      </c>
+      <c r="E2">
+        <f>Table2[reponse]*Table2[nodes]</f>
+        <v>23068910</v>
+      </c>
+      <c r="F2">
+        <f>Table2[sent to node]+Table2[sent to client]</f>
+        <v>39887348</v>
+      </c>
+      <c r="I2">
+        <f>1024*1024</f>
+        <v>1048576</v>
+      </c>
+      <c r="J2">
+        <f>(1024+1023)</f>
+        <v>2047</v>
+      </c>
+      <c r="K2">
+        <f>J2*I2</f>
+        <v>2146435072</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>12613894</v>
+      </c>
+      <c r="C3">
+        <f>Table2[request]*Table2[nodes]</f>
+        <v>25227788</v>
+      </c>
+      <c r="D3">
+        <v>11534574</v>
+      </c>
+      <c r="E3">
+        <f>Table2[reponse]*Table2[nodes]</f>
+        <v>23069148</v>
+      </c>
+      <c r="F3">
+        <f>Table2[sent to node]+Table2[sent to client]</f>
+        <v>48296936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>10511622</v>
+      </c>
+      <c r="C4">
+        <f>Table2[request]*Table2[nodes]</f>
+        <v>42046488</v>
+      </c>
+      <c r="D4">
+        <v>5767406</v>
+      </c>
+      <c r="E4">
+        <f>Table2[reponse]*Table2[nodes]</f>
+        <v>23069624</v>
+      </c>
+      <c r="F4">
+        <f>Table2[sent to node]+Table2[sent to client]</f>
+        <v>65116112</v>
+      </c>
+      <c r="I4">
+        <f>(1024*1024)*2</f>
+        <v>2097152</v>
+      </c>
+      <c r="J4">
+        <v>2148532224</v>
+      </c>
+      <c r="K4">
+        <f>K2/J4</f>
+        <v>0.99902391410444125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>9460486</v>
+      </c>
+      <c r="C5">
+        <f>Table2[request]*Table2[nodes]</f>
+        <v>75683888</v>
+      </c>
+      <c r="D5">
+        <v>2883822</v>
+      </c>
+      <c r="E5">
+        <f>Table2[reponse]*Table2[nodes]</f>
+        <v>23070576</v>
+      </c>
+      <c r="F5">
+        <f>Table2[sent to node]+Table2[sent to client]</f>
+        <v>98754464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f>I4/K2</f>
+        <v>9.7703957010258913E-4</v>
+      </c>
+      <c r="K6">
+        <f>2000/35</f>
+        <v>57.142857142857146</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sprawdzenie wydajnosci dla 1024 węzłów
</commit_message>
<xml_diff>
--- a/Programowanie współbieżne/resources/Zadanie 7.xlsx
+++ b/Programowanie współbieżne/resources/Zadanie 7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="6735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>węzły</t>
   </si>
@@ -44,12 +44,37 @@
   <si>
     <t>total data</t>
   </si>
+  <si>
+    <t>liczba operacji dla jednego węzła</t>
+  </si>
+  <si>
+    <t>łączna liczba operacji</t>
+  </si>
+  <si>
+    <t>liczba I/O dla jednego węzła</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>sprawność</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +100,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -185,11 +232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="503436928"/>
-        <c:axId val="503437504"/>
+        <c:axId val="507631232"/>
+        <c:axId val="507631808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="503436928"/>
+        <c:axId val="507631232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -199,12 +246,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="503437504"/>
+        <c:crossAx val="507631808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="503437504"/>
+        <c:axId val="507631808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -215,7 +262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="503436928"/>
+        <c:crossAx val="507631232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -327,11 +374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="571987008"/>
-        <c:axId val="571986432"/>
+        <c:axId val="544014912"/>
+        <c:axId val="544015488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="571987008"/>
+        <c:axId val="544014912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,12 +388,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571986432"/>
+        <c:crossAx val="544015488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="571986432"/>
+        <c:axId val="544015488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,7 +404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571987008"/>
+        <c:crossAx val="544014912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -367,6 +414,251 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>liczba węzłów vs. </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>sprawność</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sprawność</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.99902391410444125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99853658536585366</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99756335282651076</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99562256809338523</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99176356589147285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98413461538461533</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96922348484848486</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94071691176470584</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88845486111111116</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79960937499999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66634114583333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="77881344"/>
+        <c:axId val="54713664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="77881344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> węzłów</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54713664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54713664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>sprawność</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77881344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -449,6 +741,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
   <autoFilter ref="A1:C16"/>
@@ -467,15 +794,43 @@
   <tableColumns count="6">
     <tableColumn id="3" name="nodes"/>
     <tableColumn id="1" name="request"/>
-    <tableColumn id="4" name="sent to node" dataDxfId="2">
+    <tableColumn id="4" name="sent to node" dataDxfId="8">
       <calculatedColumnFormula>Table2[request]*Table2[nodes]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="reponse"/>
-    <tableColumn id="5" name="sent to client" dataDxfId="1">
+    <tableColumn id="5" name="sent to client" dataDxfId="7">
       <calculatedColumnFormula>Table2[reponse]*Table2[nodes]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="total data" dataDxfId="0">
+    <tableColumn id="6" name="total data" dataDxfId="6">
       <calculatedColumnFormula>Table2[sent to node]+Table2[sent to client]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="węzły"/>
+    <tableColumn id="2" name="liczba operacji dla jednego węzła" dataDxfId="5">
+      <calculatedColumnFormula>(1024+1023)*1024*1024/A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="łączna liczba operacji" dataDxfId="4">
+      <calculatedColumnFormula>A2*B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="liczba I/O dla jednego węzła" dataDxfId="3">
+      <calculatedColumnFormula>(1024*1024)+(1024*1024/A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="I/O" dataDxfId="2">
+      <calculatedColumnFormula>D2*A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="sprawność" dataDxfId="1">
+      <calculatedColumnFormula>C2/(C2+E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="%" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -939,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,12 +1464,369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>(1024+1023)*1024*1024/A2</f>
+        <v>2146435072</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C12" si="0">A2*B2</f>
+        <v>2146435072</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D12" si="1">(1024*1024)+(1024*1024/A2)</f>
+        <v>2097152</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E12" si="2">D2*A2</f>
+        <v>2097152</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F12" si="3">C2/(C2+E2)</f>
+        <v>0.99902391410444125</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" ref="G2:G12" si="4">F2</f>
+        <v>0.99902391410444125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="5">(1024+1023)*1024*1024/A3</f>
+        <v>1073217536</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>1572864</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>3145728</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="3"/>
+        <v>0.99853658536585366</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" si="4"/>
+        <v>0.99853658536585366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="5"/>
+        <v>536608768</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>1310720</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>5242880</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.99756335282651076</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="4"/>
+        <v>0.99756335282651076</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="5"/>
+        <v>268304384</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1179648</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>9437184</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.99562256809338523</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.99562256809338523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="5"/>
+        <v>134152192</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1114112</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>17825792</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.99176356589147285</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.99176356589147285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="5"/>
+        <v>67076096</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1081344</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>34603008</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.98413461538461533</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.98413461538461533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="5"/>
+        <v>33538048</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1064960</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>68157440</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.96922348484848486</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.96922348484848486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="5"/>
+        <v>16769024</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1056768</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>135266304</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.94071691176470584</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.94071691176470584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="5"/>
+        <v>8384512</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1052672</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>269484032</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.88845486111111116</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.88845486111111116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>512</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="5"/>
+        <v>4192256</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1050624</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>537919488</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.79960937499999996</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.79960937499999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1024</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="5"/>
+        <v>2096128</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2146435072</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1049600</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>1074790400</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66634114583333337</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.66634114583333337</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>